<commit_message>
Added Data Types & Variables - More Exercises
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals/00. Technlogies-Fundamentals-Courses-Schedules.xlsx
+++ b/Tech Module/Programming Fundamentals/00. Technlogies-Fundamentals-Courses-Schedules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
   <si>
     <t>Part I - Programming Fundamentals</t>
   </si>
@@ -380,12 +380,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -527,80 +535,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -610,76 +618,79 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1255,7 +1266,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,15 +1281,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1560,34 +1571,36 @@
         <f t="shared" si="2"/>
         <v>Team</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="53" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="34">
         <f t="shared" si="3"/>
         <v>42888</v>
       </c>
-      <c r="D13" s="16" t="str">
+      <c r="D13" s="35" t="str">
         <f>TEXT(C13,"dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="E13" s="12" t="str">
+      <c r="E13" s="36" t="str">
         <f t="shared" si="1"/>
         <v>18:00-22:00</v>
       </c>
-      <c r="F13" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Team</v>
-      </c>
-      <c r="G13" s="15"/>
+      <c r="F13" s="37" t="str">
+        <f t="shared" si="2"/>
+        <v>Team</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -2245,15 +2258,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Added some solved problems
</commit_message>
<xml_diff>
--- a/Tech Module/Programming Fundamentals/00. Technlogies-Fundamentals-Courses-Schedules.xlsx
+++ b/Tech Module/Programming Fundamentals/00. Technlogies-Fundamentals-Courses-Schedules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="117">
   <si>
     <t>Part I - Programming Fundamentals</t>
   </si>
@@ -380,12 +380,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -535,80 +543,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -618,79 +626,82 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1265,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,15 +1292,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1598,7 +1609,7 @@
         <f t="shared" si="2"/>
         <v>Team</v>
       </c>
-      <c r="G13" s="55" t="s">
+      <c r="G13" s="54" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1625,7 +1636,9 @@
         <f t="shared" si="2"/>
         <v>Nakov</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="56" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -2258,15 +2271,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>